<commit_message>
new rmd file for data processing
</commit_message>
<xml_diff>
--- a/data/isotopes_2.xlsx
+++ b/data/isotopes_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Public\Sawyer Balint\RStudio\wickford_cores\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5E99B6-62B7-4135-9AEA-795915ED7B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D25B57-34A6-4859-B335-608074655AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{1A6724B1-0FF8-4A94-B1F5-B2F3CDFAD274}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1A6724B1-0FF8-4A94-B1F5-B2F3CDFAD274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+      <selection activeCell="A74" sqref="A74:G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>